<commit_message>
rearrange code, add style
</commit_message>
<xml_diff>
--- a/CA_Clayton_2022.xlsx
+++ b/CA_Clayton_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xlsx2ixbrl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Process-XBRL-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7071900-76B0-48B3-BDC5-CF70D3D0F658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D1235-6E54-4F91-875D-8277F08E6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15180" windowHeight="12840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6930" yWindow="2175" windowWidth="21015" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="234">
   <si>
     <t>City of Clayton</t>
   </si>
@@ -508,9 +508,6 @@
     <t>acfr:Assets</t>
   </si>
   <si>
-    <t>acfr:Compensatedabsencespayablenoncurrent</t>
-  </si>
-  <si>
     <t>acfr:CurrentLiabilities</t>
   </si>
   <si>
@@ -556,9 +553,6 @@
     <t>acfr:DeferredInflowsOfResourcesPension</t>
   </si>
   <si>
-    <t>acfr:DeferredInflowsOfResourcesOPEBItems</t>
-  </si>
-  <si>
     <t>acfr:NetPensionLiability</t>
   </si>
   <si>
@@ -731,6 +725,18 @@
   </si>
   <si>
     <t>acfr:InvestmentGainsLossesModifiedAccrual</t>
+  </si>
+  <si>
+    <t>acfr:CompensatedAbsencesPayableNonCurrent</t>
+  </si>
+  <si>
+    <t>acfr:RevenueFromSpecialAssessmentsModifiedAccrual</t>
+  </si>
+  <si>
+    <t>acfr:NetChangeInFundBalance</t>
+  </si>
+  <si>
+    <t>acfr:DeferredInflowsOfResourcesOPEB</t>
   </si>
 </sst>
 </file>
@@ -892,7 +898,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -902,6 +907,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1227,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
+      <c r="A1" s="32"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1236,7 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1239,7 +1245,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1254,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1263,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>144</v>
       </c>
       <c r="B5" s="3"/>
@@ -1272,7 +1278,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1281,7 +1287,7 @@
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1296,7 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>145</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1307,7 +1313,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1324,7 +1330,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>147</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1341,7 +1347,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1358,7 +1364,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>149</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1375,7 +1381,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>150</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1392,7 +1398,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +1407,7 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>153</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1418,7 +1424,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>151</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1435,7 +1441,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>152</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1452,7 +1458,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>154</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1469,7 +1475,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>155</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1486,7 +1492,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>156</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1503,14 +1509,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="3"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
@@ -1519,8 +1525,8 @@
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
-        <v>167</v>
+      <c r="A23" s="33" t="s">
+        <v>166</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>27</v>
@@ -1536,8 +1542,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>168</v>
+      <c r="A24" s="33" t="s">
+        <v>167</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>29</v>
@@ -1553,8 +1559,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
-        <v>166</v>
+      <c r="A25" s="33" t="s">
+        <v>165</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>33</v>
@@ -1570,14 +1576,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="3"/>
       <c r="C26" s="11"/>
       <c r="D26" s="8"/>
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1586,7 +1592,7 @@
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
@@ -1595,8 +1601,8 @@
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
-        <v>169</v>
+      <c r="A29" s="33" t="s">
+        <v>168</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>37</v>
@@ -1612,8 +1618,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>170</v>
+      <c r="A30" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>38</v>
@@ -1629,8 +1635,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
-        <v>177</v>
+      <c r="A31" s="33" t="s">
+        <v>175</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>40</v>
@@ -1646,8 +1652,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>171</v>
+      <c r="A32" s="33" t="s">
+        <v>170</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>42</v>
@@ -1663,8 +1669,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>176</v>
+      <c r="A33" s="33" t="s">
+        <v>174</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>78</v>
@@ -1680,8 +1686,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
-        <v>178</v>
+      <c r="A34" s="33" t="s">
+        <v>176</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>45</v>
@@ -1697,8 +1703,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>158</v>
+      <c r="A35" s="33" t="s">
+        <v>157</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>47</v>
@@ -1714,7 +1720,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1723,8 +1729,8 @@
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>157</v>
+      <c r="A37" s="33" t="s">
+        <v>230</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>77</v>
@@ -1740,8 +1746,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
-        <v>175</v>
+      <c r="A38" s="33" t="s">
+        <v>173</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>50</v>
@@ -1757,8 +1763,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
-        <v>174</v>
+      <c r="A39" s="33" t="s">
+        <v>172</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>52</v>
@@ -1774,8 +1780,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
-        <v>179</v>
+      <c r="A40" s="33" t="s">
+        <v>177</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>54</v>
@@ -1791,8 +1797,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
-        <v>159</v>
+      <c r="A41" s="33" t="s">
+        <v>158</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -1808,8 +1814,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>160</v>
+      <c r="A42" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>58</v>
@@ -1825,14 +1831,14 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="3"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="3" t="s">
         <v>59</v>
       </c>
@@ -1841,8 +1847,8 @@
       <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
-        <v>172</v>
+      <c r="A45" s="33" t="s">
+        <v>171</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>60</v>
@@ -1858,8 +1864,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
-        <v>173</v>
+      <c r="A46" s="33" t="s">
+        <v>233</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>62</v>
@@ -1875,8 +1881,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
-        <v>165</v>
+      <c r="A47" s="33" t="s">
+        <v>164</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>66</v>
@@ -1892,14 +1898,14 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="3" t="s">
         <v>68</v>
       </c>
@@ -1908,8 +1914,8 @@
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
-        <v>164</v>
+      <c r="A50" s="33" t="s">
+        <v>163</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>69</v>
@@ -1925,8 +1931,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
-        <v>163</v>
+      <c r="A51" s="33" t="s">
+        <v>162</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>70</v>
@@ -1942,8 +1948,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
-        <v>162</v>
+      <c r="A52" s="33" t="s">
+        <v>161</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>72</v>
@@ -1959,8 +1965,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
-        <v>161</v>
+      <c r="A53" s="33" t="s">
+        <v>160</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>73</v>
@@ -1976,20 +1982,20 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="3"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="29" t="s">
+      <c r="A55" s="32"/>
+      <c r="B55" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
@@ -2029,34 +2035,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="31" t="s">
         <v>102</v>
       </c>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="31" t="s">
         <v>101</v>
       </c>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="32"/>
       <c r="D5" s="24"/>
       <c r="E5" s="23" t="s">
         <v>100</v>
@@ -2067,25 +2073,25 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>143</v>
       </c>
       <c r="I6" s="21" t="s">
@@ -2093,14 +2099,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>181</v>
+      <c r="A8" s="33" t="s">
+        <v>179</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>7</v>
@@ -2128,8 +2134,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>180</v>
+      <c r="A9" s="33" t="s">
+        <v>178</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>97</v>
@@ -2155,8 +2161,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>182</v>
+      <c r="A10" s="33" t="s">
+        <v>180</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>11</v>
@@ -2182,8 +2188,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>183</v>
+      <c r="A11" s="33" t="s">
+        <v>181</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>19</v>
@@ -2209,8 +2215,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>184</v>
+      <c r="A12" s="33" t="s">
+        <v>182</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>21</v>
@@ -2236,8 +2242,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>185</v>
+      <c r="A13" s="33" t="s">
+        <v>183</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>96</v>
@@ -2263,8 +2269,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>186</v>
+      <c r="A14" s="33" t="s">
+        <v>184</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>95</v>
@@ -2290,8 +2296,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>187</v>
+      <c r="A15" s="33" t="s">
+        <v>185</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>94</v>
@@ -2313,8 +2319,8 @@
       <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>188</v>
+      <c r="A16" s="33" t="s">
+        <v>186</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>25</v>
@@ -2342,7 +2348,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="19"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
@@ -2353,7 +2359,7 @@
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="19" t="s">
         <v>93</v>
       </c>
@@ -2368,7 +2374,7 @@
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="19" t="s">
         <v>92</v>
       </c>
@@ -2383,7 +2389,7 @@
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="19" t="s">
         <v>91</v>
       </c>
@@ -2398,8 +2404,8 @@
       <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
-        <v>189</v>
+      <c r="A21" s="33" t="s">
+        <v>187</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>37</v>
@@ -2427,8 +2433,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>194</v>
+      <c r="A22" s="33" t="s">
+        <v>192</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>90</v>
@@ -2456,8 +2462,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
-        <v>190</v>
+      <c r="A23" s="33" t="s">
+        <v>188</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>40</v>
@@ -2485,8 +2491,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>191</v>
+      <c r="A24" s="33" t="s">
+        <v>189</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>89</v>
@@ -2514,8 +2520,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
-        <v>193</v>
+      <c r="A25" s="33" t="s">
+        <v>191</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>42</v>
@@ -2543,8 +2549,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
-        <v>192</v>
+      <c r="A26" s="33" t="s">
+        <v>190</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>58</v>
@@ -2572,7 +2578,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="19"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -2583,7 +2589,7 @@
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="19" t="s">
         <v>88</v>
       </c>
@@ -2598,8 +2604,8 @@
       <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
-        <v>203</v>
+      <c r="A29" s="33" t="s">
+        <v>201</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>87</v>
@@ -2627,8 +2633,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>204</v>
+      <c r="A30" s="33" t="s">
+        <v>202</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>66</v>
@@ -2656,7 +2662,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="19"/>
       <c r="C31" s="27"/>
       <c r="D31" s="21"/>
@@ -2667,7 +2673,7 @@
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="19" t="s">
         <v>86</v>
       </c>
@@ -2682,8 +2688,8 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>200</v>
+      <c r="A33" s="33" t="s">
+        <v>198</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>85</v>
@@ -2711,8 +2717,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
-        <v>201</v>
+      <c r="A34" s="33" t="s">
+        <v>199</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>84</v>
@@ -2738,8 +2744,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>202</v>
+      <c r="A35" s="33" t="s">
+        <v>200</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>83</v>
@@ -2765,8 +2771,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
-        <v>198</v>
+      <c r="A36" s="33" t="s">
+        <v>196</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>82</v>
@@ -2792,8 +2798,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>199</v>
+      <c r="A37" s="33" t="s">
+        <v>197</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>81</v>
@@ -2819,8 +2825,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
-        <v>197</v>
+      <c r="A38" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>80</v>
@@ -2846,11 +2852,11 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>195</v>
+      <c r="A39" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>193</v>
       </c>
       <c r="C39" s="26">
         <v>6830902</v>
@@ -2873,7 +2879,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -2883,7 +2889,7 @@
       <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="19" t="s">
         <v>74</v>
       </c>
@@ -2898,7 +2904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D128B9-3C99-4CB8-94D6-1A47AE05AB64}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2914,35 +2922,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="31" t="s">
         <v>102</v>
       </c>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="31" t="s">
         <v>138</v>
       </c>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="31" t="s">
         <v>137</v>
       </c>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="23" t="s">
@@ -2957,26 +2965,26 @@
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>143</v>
       </c>
       <c r="I6" s="21" t="s">
@@ -2984,7 +2992,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="19" t="s">
         <v>136</v>
       </c>
@@ -2997,8 +3005,8 @@
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>205</v>
+      <c r="A8" s="33" t="s">
+        <v>203</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>135</v>
@@ -3026,8 +3034,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>218</v>
+      <c r="A9" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>134</v>
@@ -3055,9 +3063,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="str">
-        <f>"acfr:"&amp;SUBSTITUTE(B10," ","")</f>
-        <v>acfr:Specialparceltaxesandassessments</v>
+      <c r="A10" s="33" t="s">
+        <v>231</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>133</v>
@@ -3085,8 +3092,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>207</v>
+      <c r="A11" s="33" t="s">
+        <v>205</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>132</v>
@@ -3114,8 +3121,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>209</v>
+      <c r="A12" s="33" t="s">
+        <v>207</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>131</v>
@@ -3143,8 +3150,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>208</v>
+      <c r="A13" s="33" t="s">
+        <v>206</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>130</v>
@@ -3172,8 +3179,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>211</v>
+      <c r="A14" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>129</v>
@@ -3201,8 +3208,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>216</v>
+      <c r="A15" s="33" t="s">
+        <v>214</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>128</v>
@@ -3230,8 +3237,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>206</v>
+      <c r="A16" s="33" t="s">
+        <v>204</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>127</v>
@@ -3251,8 +3258,8 @@
       <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
-        <v>215</v>
+      <c r="A17" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>126</v>
@@ -3280,8 +3287,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>214</v>
+      <c r="A18" s="33" t="s">
+        <v>212</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>125</v>
@@ -3309,8 +3316,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
-        <v>213</v>
+      <c r="A19" s="33" t="s">
+        <v>211</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>124</v>
@@ -3338,8 +3345,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
-        <v>212</v>
+      <c r="A20" s="33" t="s">
+        <v>210</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>123</v>
@@ -3367,8 +3374,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
-        <v>217</v>
+      <c r="A21" s="33" t="s">
+        <v>215</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>122</v>
@@ -3396,8 +3403,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>210</v>
+      <c r="A22" s="33" t="s">
+        <v>208</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>121</v>
@@ -3425,7 +3432,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="19"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
@@ -3436,7 +3443,7 @@
       <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="19" t="s">
         <v>120</v>
       </c>
@@ -3449,7 +3456,7 @@
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="19" t="s">
         <v>119</v>
       </c>
@@ -3462,8 +3469,8 @@
       <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
-        <v>219</v>
+      <c r="A26" s="33" t="s">
+        <v>217</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>118</v>
@@ -3491,8 +3498,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
-        <v>220</v>
+      <c r="A27" s="33" t="s">
+        <v>218</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>117</v>
@@ -3520,8 +3527,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
-        <v>221</v>
+      <c r="A28" s="33" t="s">
+        <v>219</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>116</v>
@@ -3549,8 +3556,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
-        <v>222</v>
+      <c r="A29" s="33" t="s">
+        <v>220</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>115</v>
@@ -3578,8 +3585,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>223</v>
+      <c r="A30" s="33" t="s">
+        <v>221</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>114</v>
@@ -3607,8 +3614,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
-        <v>225</v>
+      <c r="A31" s="33" t="s">
+        <v>223</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>113</v>
@@ -3636,8 +3643,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>224</v>
+      <c r="A32" s="33" t="s">
+        <v>222</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>112</v>
@@ -3665,11 +3672,11 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>226</v>
+      <c r="A33" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>224</v>
       </c>
       <c r="C33" s="27">
         <v>-1348217</v>
@@ -3694,7 +3701,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="19" t="s">
         <v>111</v>
       </c>
@@ -3707,8 +3714,8 @@
       <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>231</v>
+      <c r="A35" s="33" t="s">
+        <v>229</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>110</v>
@@ -3736,8 +3743,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
-        <v>228</v>
+      <c r="A36" s="33" t="s">
+        <v>226</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>109</v>
@@ -3765,8 +3772,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>229</v>
+      <c r="A37" s="33" t="s">
+        <v>227</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>108</v>
@@ -3794,8 +3801,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
-        <v>230</v>
+      <c r="A38" s="33" t="s">
+        <v>228</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>107</v>
@@ -3823,9 +3830,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="str">
-        <f>"acfr:"&amp;SUBSTITUTE(B39," ","")</f>
-        <v>acfr:NetChangeinFundBalances</v>
+      <c r="A39" s="33" t="s">
+        <v>232</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>106</v>
@@ -3845,7 +3851,7 @@
       <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="19" t="s">
         <v>105</v>
       </c>
@@ -3866,8 +3872,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
-        <v>197</v>
+      <c r="A41" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>104</v>
@@ -3895,8 +3901,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>197</v>
+      <c r="A42" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
new context sheet, new d_to_i_contexts
</commit_message>
<xml_diff>
--- a/CA_Clayton_2022.xlsx
+++ b/CA_Clayton_2022.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Process-XBRL-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Update0803\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D1235-6E54-4F91-875D-8277F08E6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B9DF5CA-0766-405D-97A9-C1F13A887FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6930" yWindow="2175" windowWidth="21015" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="20715" windowHeight="11295" tabRatio="834" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
     <sheet name="GovFund Balance Sheet" sheetId="2" r:id="rId2"/>
     <sheet name="GovFund Stmt of Rev Exp and Chg" sheetId="3" r:id="rId3"/>
+    <sheet name="Prop Fund Stmt of Net Position" sheetId="4" r:id="rId4"/>
+    <sheet name="Prop Fund Stmt of Rev Exp Bal" sheetId="5" r:id="rId5"/>
+    <sheet name="Statement of Cash Flows" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="324">
   <si>
     <t>City of Clayton</t>
   </si>
@@ -737,6 +740,276 @@
   </si>
   <si>
     <t>acfr:DeferredInflowsOfResourcesOPEB</t>
+  </si>
+  <si>
+    <t>Due to other funds</t>
+  </si>
+  <si>
+    <t>acfr:DueToOthers</t>
+  </si>
+  <si>
+    <t>Current liabilities:</t>
+  </si>
+  <si>
+    <t>Depreciable assets, net</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>acfr:Land</t>
+  </si>
+  <si>
+    <t>Noncurrent assets</t>
+  </si>
+  <si>
+    <t>Current assets:</t>
+  </si>
+  <si>
+    <t>Governmental Activities - Internal Service Funds</t>
+  </si>
+  <si>
+    <t>Business-type Activities - Endeavor Hall</t>
+  </si>
+  <si>
+    <t>Proprietary Funds</t>
+  </si>
+  <si>
+    <t>Beginning of fiscal year</t>
+  </si>
+  <si>
+    <t>acfr:NetPositionAtBeginningOfPeriodAfterAdjustments</t>
+  </si>
+  <si>
+    <t>NET POSITION:</t>
+  </si>
+  <si>
+    <t>Change in Net Position</t>
+  </si>
+  <si>
+    <t>acfr:ChangesInNetPosition</t>
+  </si>
+  <si>
+    <t>Transfers in / (out)</t>
+  </si>
+  <si>
+    <t>acfr:TransfersNet</t>
+  </si>
+  <si>
+    <t>Capital contributions</t>
+  </si>
+  <si>
+    <t>acfr:ContributionsCapital</t>
+  </si>
+  <si>
+    <t>Net (loss) Before Contributions and Operating Transfers</t>
+  </si>
+  <si>
+    <t>acfr:IncomeLossBeforeCapitalContributions</t>
+  </si>
+  <si>
+    <t>Total Nonoperating Revenues (Expenses)</t>
+  </si>
+  <si>
+    <t>acfr:NonoperatingRevenuesAndExpenses</t>
+  </si>
+  <si>
+    <t>Investment income</t>
+  </si>
+  <si>
+    <t>acfr:InvestmentIncome</t>
+  </si>
+  <si>
+    <t>Gain (loss) on disposal of assets</t>
+  </si>
+  <si>
+    <t>acfr:GainLossOnSaleOfCapitalAssets</t>
+  </si>
+  <si>
+    <t>NONOPERATING REVENUES (EXPENSES)</t>
+  </si>
+  <si>
+    <t>Operating Income (Loss)</t>
+  </si>
+  <si>
+    <t>acfr:OperatingIncomeLoss</t>
+  </si>
+  <si>
+    <t>Total Operating Expenses</t>
+  </si>
+  <si>
+    <t>acfr:OperatingExpense</t>
+  </si>
+  <si>
+    <t>Depreciation and amortization</t>
+  </si>
+  <si>
+    <t>acfr:DepreciationExpense</t>
+  </si>
+  <si>
+    <t>General and administrative</t>
+  </si>
+  <si>
+    <t>acfr:ExpensesForGeneralGovernmentServices</t>
+  </si>
+  <si>
+    <t>Personnel</t>
+  </si>
+  <si>
+    <t>acfr:AllOtherPersonnel</t>
+  </si>
+  <si>
+    <t>OPERATING EXPENSES</t>
+  </si>
+  <si>
+    <t>Total Operating Revenues</t>
+  </si>
+  <si>
+    <t>acfr:OperatingRevenueCustom</t>
+  </si>
+  <si>
+    <t>Charges for current services</t>
+  </si>
+  <si>
+    <t>acfr:ChargesForServices</t>
+  </si>
+  <si>
+    <t>OPERATING REVENUES</t>
+  </si>
+  <si>
+    <t>Statement of Revenues, Expenses and Changes in Net Position</t>
+  </si>
+  <si>
+    <t>Net cash provided (used) by operating activities</t>
+  </si>
+  <si>
+    <t>acfr:NetCashProvidedByUsedInOperatingActivities</t>
+  </si>
+  <si>
+    <t>Increase (decrease) in interfund payables</t>
+  </si>
+  <si>
+    <t>acfr:IncreaseDecreaseInDueFromOtherFunds</t>
+  </si>
+  <si>
+    <t>Increase (decrease) in deposits payable</t>
+  </si>
+  <si>
+    <t>acfr:IncreaseDecreaseInDeposits</t>
+  </si>
+  <si>
+    <t>Increase (decrease) in accounts payable</t>
+  </si>
+  <si>
+    <t>acfr:IncreaseDecreaseInAccountsPayable</t>
+  </si>
+  <si>
+    <t>Changes in current assets and liabilities:</t>
+  </si>
+  <si>
+    <t>to net cash provided (used) by operating activities:</t>
+  </si>
+  <si>
+    <t>Adjustments to reconcile operating income (loss)</t>
+  </si>
+  <si>
+    <t>Operating income (loss)</t>
+  </si>
+  <si>
+    <t>OPERATING ACTIVITIES:</t>
+  </si>
+  <si>
+    <t>(LOSS) TO NET CASH PROVIDED (USED) BY</t>
+  </si>
+  <si>
+    <t>RECONCILIATION OF OPERATING INCOME</t>
+  </si>
+  <si>
+    <t>acfr:CashAndCashEquivalentsPerCashFlows</t>
+  </si>
+  <si>
+    <t>CASH AND CASH EQUIVALENTS:</t>
+  </si>
+  <si>
+    <t>Net increase (decrease) in cash and cash equivalents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	acfr:CashAndCashEquivalentsPeriodIncreaseDecrease</t>
+  </si>
+  <si>
+    <t>Net Cash provided by investing activities</t>
+  </si>
+  <si>
+    <t>acfr:NetCashProvidedByUsedInInvestingActivities</t>
+  </si>
+  <si>
+    <t>Interest received on investments</t>
+  </si>
+  <si>
+    <t>acfr:ProceedsFromInterestOnInvestments</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM INVESTING ACTIVITIES:</t>
+  </si>
+  <si>
+    <t>Net cash provided (used) by capital and related financing activities</t>
+  </si>
+  <si>
+    <t>acfr:NetCashProvidedByUsedInCapitalAndRelatedFinancingActivities</t>
+  </si>
+  <si>
+    <t>Proceeds from the sale of capital assets</t>
+  </si>
+  <si>
+    <t>acfr:ProceedsFromSalesOfCapitalAssets</t>
+  </si>
+  <si>
+    <t>Acquisition of fixed assets</t>
+  </si>
+  <si>
+    <t>acfr:PaymentsToPurchaseCapitalAssets</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM CAPITAL AND RELATED FINANCING ACTIVITIES:</t>
+  </si>
+  <si>
+    <t>Net cash provided by noncapital financing activities</t>
+  </si>
+  <si>
+    <t>acfr:NetCashProvidedByUsedInNonCapitalFinancingActivities</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM NONCAPITAL FINANCING ACTIVITIES:</t>
+  </si>
+  <si>
+    <t>Claims paid</t>
+  </si>
+  <si>
+    <t>acfr:CashPaidForClaimsPaid</t>
+  </si>
+  <si>
+    <t>Payments to employees</t>
+  </si>
+  <si>
+    <t>acfr:PaymentsToEmployees</t>
+  </si>
+  <si>
+    <t>Payments to suppliers</t>
+  </si>
+  <si>
+    <t>acfr:PaymentsToSuppliers</t>
+  </si>
+  <si>
+    <t>Receipts from customers</t>
+  </si>
+  <si>
+    <t>acfr:ProceedsFromSalesAndServices</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM OPERATING ACTIVITIES:</t>
+  </si>
+  <si>
+    <t>Statement of Cash Flows</t>
   </si>
 </sst>
 </file>
@@ -746,7 +1019,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-809]#,##0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -794,6 +1067,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -852,7 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -908,6 +1188,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1215,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -2904,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D128B9-3C99-4CB8-94D6-1A47AE05AB64}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -3948,4 +4238,1062 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1472389-47EF-405E-8CCC-659CBF543E59}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
+      <c r="B7" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="26">
+        <v>460441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="27">
+        <v>167738</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" s="27">
+        <v>841465</v>
+      </c>
+      <c r="D11" s="27">
+        <v>540610</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="27">
+        <v>1009203</v>
+      </c>
+      <c r="D12" s="27">
+        <v>1001051</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="27">
+        <v>2671</v>
+      </c>
+      <c r="D15" s="28">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="27">
+        <v>5500</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="27">
+        <v>120893</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="27">
+        <v>129064</v>
+      </c>
+      <c r="D19" s="28">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="27">
+        <v>1009203</v>
+      </c>
+      <c r="D21" s="27">
+        <v>540610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="27">
+        <v>-129064</v>
+      </c>
+      <c r="D22" s="27">
+        <v>460126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="26">
+        <v>880139</v>
+      </c>
+      <c r="D23" s="26">
+        <v>1000736</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561EF3A4-62DC-4CA7-A3A2-3DAB05769638}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="16" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="31" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="26">
+        <v>16847</v>
+      </c>
+      <c r="D7" s="26">
+        <v>111900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" s="27">
+        <v>16847</v>
+      </c>
+      <c r="D8" s="27">
+        <v>111900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="27">
+        <v>4833</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="27">
+        <v>26989</v>
+      </c>
+      <c r="D11" s="27">
+        <v>8564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="27">
+        <v>28872</v>
+      </c>
+      <c r="D12" s="27">
+        <v>100425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C13" s="27">
+        <v>60694</v>
+      </c>
+      <c r="D13" s="27">
+        <v>108989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" s="27">
+        <v>-43847</v>
+      </c>
+      <c r="D14" s="27">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="27">
+        <v>6958</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="27">
+        <v>-14675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="27">
+        <v>-7717</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="38">
+        <v>-43847</v>
+      </c>
+      <c r="D19" s="38">
+        <v>-4806</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="27">
+        <v>-43847</v>
+      </c>
+      <c r="D22" s="27">
+        <v>-4806</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="27">
+        <v>923986</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1005542</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="26">
+        <v>880139</v>
+      </c>
+      <c r="D25" s="26">
+        <v>1000736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F974A34E-AF89-4E55-8474-086D4B24BD38}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="19"/>
+    <col min="8" max="8" width="21.42578125" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="26">
+        <v>20847</v>
+      </c>
+      <c r="D7" s="26">
+        <v>111900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="27">
+        <v>-24734</v>
+      </c>
+      <c r="D8" s="27">
+        <v>-4001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="27">
+        <v>-4833</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="27">
+        <v>-4428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="27">
+        <v>-8720</v>
+      </c>
+      <c r="D11" s="27">
+        <v>103471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="27">
+        <v>8720</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C14" s="27">
+        <v>8720</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="27">
+        <v>-153184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="27">
+        <v>6958</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="27">
+        <v>-146226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="27">
+        <v>-14675</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="27">
+        <v>-14675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="27">
+        <v>-57430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="27">
+        <v>517871</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="26">
+        <v>460441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="26">
+        <v>-43847</v>
+      </c>
+      <c r="D29" s="26">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C32" s="27">
+        <v>28872</v>
+      </c>
+      <c r="D32" s="27">
+        <v>100425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C34" s="27">
+        <v>2255</v>
+      </c>
+      <c r="D34" s="28">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="C35" s="27">
+        <v>4000</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="C37" s="26">
+        <v>-8720</v>
+      </c>
+      <c r="D37" s="26">
+        <v>103471</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
+      <c r="B39" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>